<commit_message>
update merger and order
</commit_message>
<xml_diff>
--- a/data/reporting/End_User_To_Course_Report.xlsx
+++ b/data/reporting/End_User_To_Course_Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="465" windowWidth="17955" windowHeight="11985"/>
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="COURSE REPORT" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'COURSE REPORT'!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -127,12 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -149,10 +149,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,17 +467,17 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="12" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" customWidth="1"/>
     <col min="9" max="9" width="37.7109375" customWidth="1"/>
@@ -479,22 +488,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -509,7 +518,7 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -520,153 +529,154 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="2"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="6"/>
+      <c r="A2" s="11"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="2"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="6"/>
+      <c r="A3" s="11"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="2"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="6"/>
+      <c r="A4" s="11"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="2"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="6"/>
+      <c r="A5" s="11"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="2"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="6"/>
+      <c r="A6" s="11"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="2"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6"/>
+      <c r="A7" s="11"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="2"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="6"/>
+      <c r="A8" s="11"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="2"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="6"/>
+      <c r="A9" s="11"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="2"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="6"/>
+      <c r="A10" s="11"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="2"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="6"/>
+      <c r="A11" s="11"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="2"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="6"/>
+      <c r="A12" s="11"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="2"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="6"/>
+      <c r="A13" s="11"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="2"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="6"/>
+      <c r="A14" s="11"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="2"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="6"/>
+      <c r="A15" s="11"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="2"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="6"/>
+      <c r="A16" s="11"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:10" hidden="1">
-      <c r="A17" s="2"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="2"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="4"/>
+      <c r="A18" s="11"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="2"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
+      <c r="A19" s="11"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="2"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="2"/>
+      <c r="A21" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix issues: DURM-144, DURM-146
</commit_message>
<xml_diff>
--- a/data/reporting/End_User_To_Course_Report.xlsx
+++ b/data/reporting/End_User_To_Course_Report.xlsx
@@ -160,7 +160,892 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="220">
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <sz val="12"/>
@@ -574,131 +1459,66 @@
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
     </pivotField>
   </pivotFields>
   <rowFields count="13">
@@ -740,176 +1560,176 @@
     <i/>
   </colItems>
   <formats count="55">
-    <format dxfId="54">
+    <format dxfId="219">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="218">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="217">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="216">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="215">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="214">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="213">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="212">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="211">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="210">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="209">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="208">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="207">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="206">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="205">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="204">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="203">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="202">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="201">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="200">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="199">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="198">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="197">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="196">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="195">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="194">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="193">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="192">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="191">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="190">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="189">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="188">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="187">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="186">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="185">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="184">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="183">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="182">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="181">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="180">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="179">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="178">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="177">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="176">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="175">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="174">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="173">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="172">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="171">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="170">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="169">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="168">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="167">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="166">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="165">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="1" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
   </extLst>
 </pivotTableDefinition>

</xml_diff>

<commit_message>
Update template Training course report
</commit_message>
<xml_diff>
--- a/data/reporting/End_User_To_Course_Report.xlsx
+++ b/data/reporting/End_User_To_Course_Report.xlsx
@@ -1134,11 +1134,11 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="17" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="24" style="7" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="13.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="17" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="24" style="7" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="54.5703125" bestFit="1" customWidth="1"/>

</xml_diff>